<commit_message>
upload labnote up to oligomer assembly workflow
</commit_message>
<xml_diff>
--- a/labnote/001_oligo_assembly_test_GFP-mCherry/resources/oligopool_order/oligo_order_251015_sfGFP_mCherry_58-61Tm.xlsx
+++ b/labnote/001_oligo_assembly_test_GFP-mCherry/resources/oligopool_order/oligo_order_251015_sfGFP_mCherry_58-61Tm.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\workspace\labnote\labnote\002_251013_oligo_assembly_test_GFP-mCherry\resources\oligopool_order\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\workspace\labnote\labnote\oligo_assembly_SOP\labnote\001_oligo_assembly_test_GFP-mCherry\resources\oligopool_order\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7027C127-314F-4262-AFC5-BE3990EE9B24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C208F6F-DAE5-4075-ADCF-F0CD0F42BE0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5657" yWindow="1646" windowWidth="26494" windowHeight="15617" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57480" yWindow="-30" windowWidth="16440" windowHeight="28320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -162,6 +162,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="178" formatCode="0.0"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -214,7 +217,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -519,10 +522,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F33"/>
+  <dimension ref="A1:F34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.600000000000001" x14ac:dyDescent="0.55000000000000004"/>
@@ -1067,6 +1070,12 @@
         <v>58.896551724137929</v>
       </c>
     </row>
+    <row r="34" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="C34" s="3">
+        <f>AVERAGE(C2:C31)</f>
+        <v>79.466666666666669</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>